<commit_message>
Updated CRUD and UC Desc to add password
Added UC for updateing passwords and changed old update UCs. Also added
to CRUD analysis.
</commit_message>
<xml_diff>
--- a/CRUD Analysis.xlsx
+++ b/CRUD Analysis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="168">
   <si>
     <t>Use Case</t>
   </si>
@@ -380,55 +380,28 @@
     <t>Update_Assessment</t>
   </si>
   <si>
-    <t>2.11</t>
-  </si>
-  <si>
     <t>View_Assessment</t>
-  </si>
-  <si>
-    <t>2.12</t>
   </si>
   <si>
     <t>Delete_Assessment</t>
   </si>
   <si>
-    <t>2.13</t>
-  </si>
-  <si>
     <t>Register_Assessment_Allocation</t>
-  </si>
-  <si>
-    <t>2.14</t>
   </si>
   <si>
     <t>Update_Assessment_Allocation</t>
   </si>
   <si>
-    <t>2.15</t>
-  </si>
-  <si>
     <t>View_Assessment_Allocation</t>
-  </si>
-  <si>
-    <t>2.16</t>
   </si>
   <si>
     <t>Delete_Assessment_Allocation</t>
   </si>
   <si>
-    <t>2.17</t>
-  </si>
-  <si>
     <t>Register_Team_Allocation</t>
   </si>
   <si>
-    <t>2.18</t>
-  </si>
-  <si>
     <t>View_Team_Allocation</t>
-  </si>
-  <si>
-    <t>2.19</t>
   </si>
   <si>
     <t>Update_Team_Allocation</t>
@@ -514,12 +487,45 @@
   <si>
     <t>Create_Meeting_Type</t>
   </si>
+  <si>
+    <t>Update_Admin_Password</t>
+  </si>
+  <si>
+    <t>Update_Supervisor_Password</t>
+  </si>
+  <si>
+    <t>Update_Convenor_Password</t>
+  </si>
+  <si>
+    <t>Update_Student_Password</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>View_Team_Assessment</t>
+  </si>
+  <si>
+    <t>Register_Role_Type</t>
+  </si>
+  <si>
+    <t>View_Role_Type</t>
+  </si>
+  <si>
+    <t>Update_Role_Type</t>
+  </si>
+  <si>
+    <t>Delete_Role_Type</t>
+  </si>
+  <si>
+    <t>RoleType</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -558,6 +564,17 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -619,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -684,6 +701,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,6 +711,33 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -998,10 +1043,10 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:R1"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1060,7 @@
     <col min="8" max="8" width="20.5703125" customWidth="1"/>
     <col min="9" max="9" width="7.28515625" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="5" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" customWidth="1"/>
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
@@ -1028,34 +1073,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="T1" s="24" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="T1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
@@ -1091,8 +1136,8 @@
       <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>13</v>
+      <c r="K2" s="37" t="s">
+        <v>167</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>14</v>
@@ -1683,8 +1728,8 @@
       <c r="A19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>62</v>
+      <c r="B19" s="36" t="s">
+        <v>163</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1715,8 +1760,8 @@
       <c r="A20" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>64</v>
+      <c r="B20" s="36" t="s">
+        <v>164</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1747,8 +1792,8 @@
       <c r="A21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>66</v>
+      <c r="B21" s="36" t="s">
+        <v>165</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1779,8 +1824,8 @@
       <c r="A22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>68</v>
+      <c r="B22" s="36" t="s">
+        <v>166</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2348,11 +2393,11 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>101</v>
+      <c r="A39" s="32">
+        <v>1.37</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>102</v>
+      <c r="B39" s="29" t="s">
+        <v>157</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2360,17 +2405,13 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="5" t="s">
-        <v>33</v>
+      <c r="I39" s="5"/>
+      <c r="J39" s="30" t="s">
+        <v>30</v>
       </c>
-      <c r="J39" s="2"/>
-      <c r="K39" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="K39" s="5"/>
       <c r="L39" s="5"/>
-      <c r="M39" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="M39" s="5"/>
       <c r="N39" s="5"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
@@ -2384,11 +2425,11 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>103</v>
+      <c r="A40" s="33" t="s">
+        <v>101</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2399,13 +2440,13 @@
       <c r="I40" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J40" s="2"/>
+      <c r="J40" s="5"/>
       <c r="K40" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L40" s="5"/>
       <c r="M40" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -2420,11 +2461,11 @@
       <c r="Z40" s="2"/>
     </row>
     <row r="41" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>105</v>
+      <c r="A41" s="33" t="s">
+        <v>103</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -2435,13 +2476,13 @@
       <c r="I41" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J41" s="2"/>
+      <c r="J41" s="5"/>
       <c r="K41" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L41" s="5"/>
       <c r="M41" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -2456,11 +2497,11 @@
       <c r="Z41" s="2"/>
     </row>
     <row r="42" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>107</v>
+      <c r="A42" s="33" t="s">
+        <v>105</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2471,13 +2512,13 @@
       <c r="I42" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J42" s="2"/>
+      <c r="J42" s="5"/>
       <c r="K42" s="5" t="s">
         <v>33</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -2492,27 +2533,29 @@
       <c r="Z42" s="2"/>
     </row>
     <row r="43" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>109</v>
+      <c r="A43" s="33" t="s">
+        <v>107</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>110</v>
+      <c r="B43" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="J43" s="5"/>
-      <c r="K43" s="2"/>
+      <c r="K43" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
+      <c r="M43" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
@@ -2526,22 +2569,22 @@
       <c r="Z43" s="2"/>
     </row>
     <row r="44" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>111</v>
+      <c r="A44" s="33" t="s">
+        <v>109</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="5"/>
       <c r="D44" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="2"/>
@@ -2560,22 +2603,22 @@
       <c r="Z44" s="2"/>
     </row>
     <row r="45" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>113</v>
+      <c r="A45" s="33" t="s">
+        <v>111</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
-      <c r="C45" s="2"/>
+      <c r="C45" s="5"/>
       <c r="D45" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="2"/>
@@ -2594,22 +2637,22 @@
       <c r="Z45" s="2"/>
     </row>
     <row r="46" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>115</v>
+      <c r="A46" s="33" t="s">
+        <v>113</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
-      <c r="C46" s="2"/>
+      <c r="C46" s="5"/>
       <c r="D46" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="2"/>
@@ -2628,24 +2671,24 @@
       <c r="Z46" s="2"/>
     </row>
     <row r="47" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>117</v>
+      <c r="A47" s="33" t="s">
+        <v>115</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6" t="s">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="6" t="s">
-        <v>26</v>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5" t="s">
+        <v>36</v>
       </c>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
+      <c r="J47" s="5"/>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
@@ -2662,18 +2705,18 @@
       <c r="Z47" s="2"/>
     </row>
     <row r="48" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>119</v>
+      <c r="A48" s="33" t="s">
+        <v>117</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>120</v>
+      <c r="B48" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
@@ -2696,18 +2739,18 @@
       <c r="Z48" s="2"/>
     </row>
     <row r="49" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>121</v>
+      <c r="A49" s="33" t="s">
+        <v>119</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>122</v>
+      <c r="B49" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
@@ -2730,18 +2773,18 @@
       <c r="Z49" s="2"/>
     </row>
     <row r="50" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
-        <v>123</v>
+      <c r="A50" s="31">
+        <v>2.11</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
@@ -2764,26 +2807,24 @@
       <c r="Z50" s="2"/>
     </row>
     <row r="51" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>125</v>
+      <c r="A51" s="31">
+        <v>2.12</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="5" t="s">
+      <c r="C51" s="6"/>
+      <c r="D51" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5" t="s">
-        <v>33</v>
+      <c r="E51" s="6" t="s">
+        <v>36</v>
       </c>
-      <c r="H51" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="5"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="2"/>
@@ -2800,11 +2841,11 @@
       <c r="Z51" s="2"/>
     </row>
     <row r="52" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>127</v>
+      <c r="A52" s="31">
+        <v>2.13</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2816,7 +2857,7 @@
         <v>33</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="5"/>
@@ -2836,11 +2877,11 @@
       <c r="Z52" s="2"/>
     </row>
     <row r="53" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
-        <v>129</v>
+      <c r="A53" s="31">
+        <v>2.14</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>130</v>
+      <c r="B53" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2852,7 +2893,7 @@
         <v>33</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="5"/>
@@ -2872,11 +2913,11 @@
       <c r="Z53" s="2"/>
     </row>
     <row r="54" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>131</v>
+      <c r="A54" s="31">
+        <v>2.15</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>132</v>
+      <c r="B54" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2888,7 +2929,7 @@
         <v>33</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="5"/>
@@ -2908,30 +2949,30 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>133</v>
+      <c r="A55" s="31">
+        <v>2.16</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F55" s="2"/>
       <c r="G55" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H55" s="2"/>
+      <c r="H55" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
-      <c r="M55" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N55" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
       <c r="Q55" s="2"/>
@@ -2944,11 +2985,11 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>135</v>
+      <c r="A56" s="31">
+        <v>2.17</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>136</v>
+      <c r="B56" s="10" t="s">
+        <v>127</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -2966,7 +3007,7 @@
         <v>33</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
@@ -2980,11 +3021,11 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>137</v>
+      <c r="A57" s="31">
+        <v>2.1800000000000002</v>
       </c>
-      <c r="B57" s="7" t="s">
-        <v>138</v>
+      <c r="B57" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -3002,7 +3043,7 @@
         <v>33</v>
       </c>
       <c r="N57" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
@@ -3016,11 +3057,11 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>139</v>
+      <c r="A58" s="31">
+        <v>2.19</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>140</v>
+      <c r="B58" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -3031,14 +3072,14 @@
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
+      <c r="J58" s="5"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="5" t="s">
         <v>33</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
@@ -3052,29 +3093,31 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>141</v>
+      <c r="A59" s="33" t="s">
+        <v>130</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>142</v>
+      <c r="B59" s="10" t="s">
+        <v>131</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N59" s="5"/>
-      <c r="O59" s="5" t="s">
-        <v>33</v>
+      <c r="N59" s="5" t="s">
+        <v>36</v>
       </c>
+      <c r="O59" s="5"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="T59" s="2"/>
@@ -3086,29 +3129,27 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>143</v>
+      <c r="A60" s="32">
+        <v>2.21</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>144</v>
+      <c r="B60" s="29" t="s">
+        <v>159</v>
       </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
-      <c r="M60" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="M60" s="5"/>
       <c r="N60" s="5"/>
-      <c r="O60" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="O60" s="5"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="T60" s="2"/>
@@ -3120,20 +3161,20 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>145</v>
+      <c r="A61" s="33" t="s">
+        <v>132</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
       <c r="M61" s="5" t="s">
@@ -3141,7 +3182,7 @@
       </c>
       <c r="N61" s="5"/>
       <c r="O61" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
@@ -3154,20 +3195,20 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>147</v>
+      <c r="A62" s="33" t="s">
+        <v>134</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="5" t="s">
@@ -3175,7 +3216,7 @@
       </c>
       <c r="N62" s="5"/>
       <c r="O62" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
@@ -3188,11 +3229,11 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>149</v>
+      <c r="A63" s="33" t="s">
+        <v>136</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3204,16 +3245,14 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5" t="s">
+      <c r="M63" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="N63" s="5"/>
       <c r="O63" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
-      <c r="P63" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="P63" s="5"/>
       <c r="Q63" s="2"/>
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
@@ -3224,11 +3263,11 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
-        <v>151</v>
+      <c r="A64" s="33" t="s">
+        <v>138</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -3240,16 +3279,14 @@
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5" t="s">
+      <c r="M64" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="N64" s="5"/>
       <c r="O64" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
-      <c r="P64" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="P64" s="5"/>
       <c r="Q64" s="2"/>
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
@@ -3260,11 +3297,11 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>153</v>
+      <c r="A65" s="34">
+        <v>3.5</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>154</v>
+      <c r="B65" s="29" t="s">
+        <v>158</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -3273,19 +3310,15 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
+      <c r="J65" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="5"/>
-      <c r="N65" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O65" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P65" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5"/>
+      <c r="P65" s="5"/>
       <c r="Q65" s="2"/>
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
@@ -3296,11 +3329,11 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
-        <v>155</v>
+      <c r="A66" s="33" t="s">
+        <v>140</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -3320,7 +3353,7 @@
         <v>33</v>
       </c>
       <c r="P66" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="Q66" s="2"/>
       <c r="T66" s="2"/>
@@ -3332,8 +3365,12 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="10"/>
-      <c r="B67" s="10"/>
+      <c r="A67" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>143</v>
+      </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -3341,13 +3378,19 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
+      <c r="J67" s="5"/>
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
+      <c r="N67" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O67" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P67" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="Q67" s="2"/>
       <c r="T67" s="2"/>
       <c r="U67" s="2"/>
@@ -3358,8 +3401,12 @@
       <c r="Z67" s="2"/>
     </row>
     <row r="68" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="10"/>
-      <c r="B68" s="10"/>
+      <c r="A68" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>145</v>
+      </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -3367,13 +3414,19 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
+      <c r="J68" s="5"/>
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
       <c r="M68" s="2"/>
-      <c r="N68" s="2"/>
-      <c r="O68" s="2"/>
-      <c r="P68" s="2"/>
+      <c r="N68" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O68" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P68" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="Q68" s="2"/>
       <c r="T68" s="2"/>
       <c r="U68" s="2"/>
@@ -3384,8 +3437,12 @@
       <c r="Z68" s="2"/>
     </row>
     <row r="69" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="10"/>
-      <c r="B69" s="10"/>
+      <c r="A69" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>147</v>
+      </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -3393,13 +3450,19 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
-      <c r="J69" s="2"/>
+      <c r="J69" s="5"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
       <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
-      <c r="O69" s="2"/>
-      <c r="P69" s="2"/>
+      <c r="N69" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O69" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P69" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="Q69" s="2"/>
       <c r="T69" s="2"/>
       <c r="U69" s="2"/>
@@ -3410,16 +3473,24 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10"/>
+      <c r="A70" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="B70" s="36" t="s">
+        <v>162</v>
+      </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
+      <c r="E70" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F70" s="35"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
+      <c r="H70" s="35" t="s">
+        <v>33</v>
+      </c>
       <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
+      <c r="J70" s="30"/>
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
@@ -3436,23 +3507,30 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="10"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="2"/>
-      <c r="N71" s="2"/>
-      <c r="O71" s="2"/>
-      <c r="P71" s="2"/>
-      <c r="Q71" s="2"/>
+      <c r="A71" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="B71" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="30"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+      <c r="O71" s="5"/>
+      <c r="P71" s="5"/>
+      <c r="Q71" s="5"/>
+      <c r="R71" s="24"/>
       <c r="T71" s="2"/>
       <c r="U71" s="2"/>
       <c r="V71" s="2"/>
@@ -27720,12 +27798,16 @@
       <c r="Z1004" s="2"/>
     </row>
   </sheetData>
+  <sortState ref="A40:R70">
+    <sortCondition ref="A70"/>
+  </sortState>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="T1:W1"/>
     <mergeCell ref="C1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27761,28 +27843,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="24" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
       <c r="S1" s="12"/>
       <c r="T1" s="12"/>
       <c r="U1" s="12"/>
@@ -27827,7 +27909,7 @@
         <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>17</v>
@@ -27982,13 +28064,13 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="27" t="s">
-        <v>158</v>
+      <c r="J6" s="28" t="s">
+        <v>149</v>
       </c>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -28017,11 +28099,11 @@
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -28412,7 +28494,7 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="14" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -28454,7 +28536,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="15" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -28808,7 +28890,7 @@
         <v>2.11</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -28846,7 +28928,7 @@
         <v>2.12</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -28884,7 +28966,7 @@
         <v>2.13</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -28922,7 +29004,7 @@
         <v>2.14</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -28960,7 +29042,7 @@
         <v>2.15</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -28998,7 +29080,7 @@
         <v>2.16</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -29036,7 +29118,7 @@
         <v>3.1</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -29072,7 +29154,7 @@
         <v>3.2</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -29108,7 +29190,7 @@
         <v>3.3</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -29144,7 +29226,7 @@
         <v>3.4</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -29180,7 +29262,7 @@
         <v>3.5</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -29214,7 +29296,7 @@
         <v>3.6</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>33</v>
@@ -29288,7 +29370,7 @@
         <v>4.2</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -29322,7 +29404,7 @@
         <v>4.3</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -29358,7 +29440,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -29393,7 +29475,7 @@
         <v>4.5</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -29429,7 +29511,7 @@
     <row r="46" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="21"/>
       <c r="B46" s="9" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -29557,7 +29639,7 @@
     <row r="50" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="22"/>
       <c r="B50" s="9" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>

</xml_diff>